<commit_message>
Testování výstupů a zpracovani dat z KN.
</commit_message>
<xml_diff>
--- a/GIS2/vystup.xlsx
+++ b/GIS2/vystup.xlsx
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>55</v>
+        <v>661</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -491,17 +491,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>69/26</t>
+          <t>st. 110</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Říčany-Radošovice</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>č. 69/26 Říčany-Radošovice</t>
+          <t>stavební č. 110 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -515,11 +515,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>56</v>
+        <v>662</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,17 +529,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>st. 736</t>
+          <t>172/40</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Říčany-Radošovice</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>stavební č. 736 Říčany-Radošovice (součástí je stavba č.p. 366, čst obce Radošovice)</t>
+          <t>č. 172/40 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -547,17 +547,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>57</v>
+        <v>663</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>92/13</t>
+          <t>st. 602</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Říčany-Radošovice</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>č. 92/13 Říčany-Radošovice</t>
+          <t>stavební č. 602 Nová Ves u Prahy (součástí je stavba č.p. 519, čst obce Nová Ves)</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -585,13 +585,13 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>58</v>
+        <v>664</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -605,17 +605,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>561/6</t>
+          <t>173/122</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Říčany-Radošovice</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>č. 561/6 Říčany-Radošovice</t>
+          <t>č. 173/122 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -629,7 +629,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>63</v>
+        <v>665</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -643,17 +643,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>263/2</t>
+          <t>173/127</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>č. 263/2 Těptín</t>
+          <t>č. 173/127 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -667,11 +667,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>64</v>
+        <v>16796</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -681,17 +681,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>516/3</t>
+          <t>st. 323</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>č. 516/3 Těptín</t>
+          <t>stavební č. 323 Nová Ves u Prahy (součástí je stavba č.p. 247, čst obce Nová Ves)</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -699,17 +699,17 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>65</v>
+        <v>16797</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -719,17 +719,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>st. 1105</t>
+          <t>95/66</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>jednotka č. 280014, byt v budově č.p. 28, část obce Kamenice, na parcele st. 1105 Těptín, podíl na společných částech domu a pozemku 381/6380</t>
+          <t>č. 95/66 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -737,17 +737,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>66</v>
+        <v>16798</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>jednotka</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -757,17 +757,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>619/1</t>
+          <t>st. 298</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>č. 619/1 Těptín</t>
+          <t>jednotka č. 2650083, byt v budově č.p. 265, část obce Nová Ves, na parcele st. 298 Nová Ves u Prahy, podíl na společných částech domu a pozemku 620/1984</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -775,13 +775,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>jednotka na parcele s prefixem st. + KU</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>67</v>
+        <v>16799</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -795,17 +795,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>725/28</t>
+          <t>95/218</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>č. 725/28 Těptín</t>
+          <t>č. 95/218 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -819,11 +819,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>68</v>
+        <v>16800</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -833,17 +833,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>st. 1603</t>
+          <t>95/131</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Těptín</t>
+          <t>Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>stavební č. 1603 Těptín (součástí je stavba č.p. 2833, čst obce Těptín)</t>
+          <t>č. 95/131 Nová Ves u Prahy</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Upravena FCE na hledani kodu ku v Praze pres kombinaci obec + ku
</commit_message>
<xml_diff>
--- a/GIS2/vystup.xlsx
+++ b/GIS2/vystup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>661</v>
+        <v>58842</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -486,22 +486,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>st. 110</t>
+          <t>1044/2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>stavební č. 110 Nová Ves u Prahy</t>
+          <t>č. 1044/2 Libuš</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -515,31 +515,31 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>662</v>
+        <v>58841</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>172/40</t>
+          <t>1044/4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>č. 172/40 Nová Ves u Prahy</t>
+          <t>č. 1044/4 Libuš (součástí je stavba č.p. 957, čst obce Libuš)</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -547,37 +547,37 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>663</v>
+        <v>58840</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>st. 602</t>
+          <t>1087/2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>stavební č. 602 Nová Ves u Prahy (součástí je stavba č.p. 519, čst obce Nová Ves)</t>
+          <t>č. 1087/2 Libuš</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -585,13 +585,13 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>664</v>
+        <v>58839</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -600,22 +600,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>173/122</t>
+          <t>1088</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>č. 173/122 Nová Ves u Prahy</t>
+          <t>č. 1088 Libuš</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -629,31 +629,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>665</v>
+        <v>58838</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>173/127</t>
+          <t>1087/1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>č. 173/127 Nová Ves u Prahy</t>
+          <t>č. 1087/1 Libuš (součástí je stavba č.p. 435, čst obce Libuš)</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -661,37 +661,37 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16796</v>
+        <v>58837</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>st. 323</t>
+          <t>546/1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>stavební č. 323 Nová Ves u Prahy (součástí je stavba č.p. 247, čst obce Nová Ves)</t>
+          <t>č. 546/1 Libuš</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -699,13 +699,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16797</v>
+        <v>58836</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -714,22 +714,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>95/66</t>
+          <t>546/3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>č. 95/66 Nová Ves u Prahy</t>
+          <t>č. 546/3 Libuš</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -743,31 +743,31 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>16798</v>
+        <v>58835</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>st. 298</t>
+          <t>546/2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>jednotka č. 2650083, byt v budově č.p. 265, část obce Nová Ves, na parcele st. 298 Nová Ves u Prahy, podíl na společných částech domu a pozemku 620/1984</t>
+          <t>č. 546/2 Libuš (součástí je stavba budova bez čp/če, jiná stavba)</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -775,37 +775,37 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>16799</v>
+        <v>58834</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>95/218</t>
+          <t>546/4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Libuš</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>č. 95/218 Nová Ves u Prahy</t>
+          <t>č. 546/4 Libuš (součástí je stavba budova bez čp/če, jiná stavba)</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -813,13 +813,13 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16800</v>
+        <v>58833</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -828,28 +828,2042 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Praha-východ</t>
+          <t>Hlavní město Praha</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>95/131</t>
+          <t>835/84</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Nová Ves u Prahy</t>
+          <t>Písnice</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>č. 95/131 Nová Ves u Prahy</t>
+          <t>č. 835/84 Písnice</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
       <c r="H11" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>58832</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>761</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>č. 761 Písnice</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>58831</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>760</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>č. 760 Písnice (součástí je stavba č.p. 329, čst obce Písnice)</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>910/2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>jednotka na parcele bez prefixu st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>910/3</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>910/4</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>910/5</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>910/6</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>58830</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>910/7</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Písnice</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>58829</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2197/2</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>č. 2197/2 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>58828</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>st. 500</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>stavební č. 500 Ledeč nad Sázavou (součástí je stavba č.p. 117, čst obce Horní Ledeč)</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>58827</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>st. 825</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>jednotka č. 6450002, byt v budově č.p. 645, 646, část obce Ledeč nad Sázavou, na parcele st. 825 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 237/12278</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>jednotka na parcele s prefixem st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>58826</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2090/24</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>č. 2090/24 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>58825</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>st. 614</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>jednotka č. 5540005, byt v budově č.p. 553, 554, část obce Ledeč nad Sázavou, na parcele st. 614 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 629/8741</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>jednotka na parcele s prefixem st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>58824</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>st. 722</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>jednotka č. 6700007, byt v budově č.p. 670, část obce Ledeč nad Sázavou, na parcele st. 722 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 52/1000</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>jednotka na parcele s prefixem st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>58823</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>823/5</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>č. 823/5 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>58822</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>823/25</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>č. 823/25 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>58821</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>823/32</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>č. 823/32 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>58820</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>st. 1640</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>stavební č. 1640 Ledeč nad Sázavou (součástí je stavba budova bez čp/če, garáž)</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>58819</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>st. 710/2</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>stavební č. 710/2 Ledeč nad Sázavou (součástí je stavba budova bez čp/če, jiná stavba)</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>58818</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>st. 710/1</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>stavební č. 710/1 Ledeč nad Sázavou (součástí je stavba č.p. 674, čst obce Ledeč nad Sázavou)</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>58817</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>964</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>č. 964 Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>58816</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Havlíčkův Brod</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>st. 601</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Ledeč nad Sázavou</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>jednotka č. 5560004, byt v budově č.p. 557, 555, 556, část obce Ledeč nad Sázavou, na parcele st. 601 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 519/9693</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>jednotka na parcele s prefixem st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>58815</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>429/48</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>jednotka č. 9860006, garáž v budově č.p. 986, část obce Libuš, na parcele 429/48 Libuš, podíl na společných částech domu a pozemku 184814/679789</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>jednotka na parcele bez prefixu st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>58814</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>429/48</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>jednotka č. 9860410, byt v budově č.p. 986, část obce Libuš, na parcele 429/48 Libuš, podíl na společných částech domu a pozemku 5732/679789</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>jednotka na parcele bez prefixu st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>58813</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1123/116</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>č. 1123/116 Libuš</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>58812</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1123/76</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>č. 1123/76 Libuš</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>58811</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>1123/73</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>č. 1123/73 Libuš</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>58810</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1123/120</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>č. 1123/120 Libuš</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>58809</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>1123/118</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>č. 1123/118 Libuš</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>58808</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1123/119</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>č. 1123/119 Libuš</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>58807</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1123/117</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Libuš</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>č. 1123/117 Libuš</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>58806</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2382/8</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>č. 2382/8 Kunratice</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>58805</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2342/27</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>č. 2342/27 Kunratice</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>58804</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2342/30</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>č. 2342/30 Kunratice</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>58803</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2342/28</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>č. 2342/28 Kunratice</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>58802</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2342/29</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>č. 2342/29 Kunratice</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>58801</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2342/31</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>č. 2342/31 Kunratice</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>58800</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2342/27</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>jednotka na parcele bez prefixu st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>58800</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2342/28</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>58800</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2342/29</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>58800</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2342/30</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>58800</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2342/31</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>58799</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2342/27</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>jednotka na parcele bez prefixu st. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>58799</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2342/28</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>58799</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2342/29</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>58799</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2342/30</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>58799</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>jednotka</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2342/31</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>více parcel oddělených čárkou</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58798</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>1433/13</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>č. 1433/13 Kunratice</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58797</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>1433/12</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>č. 1433/12 Kunratice</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>58796</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>59/12</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>č. 59/12 Kunratice</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>číslo a KU za ním</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>58795</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>59/45</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>č. 59/45 Kunratice (součástí je stavba č.p. 1045, čst obce Kunratice)</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>č. + KU</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>58794</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>budova</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>267/9</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>budova bez čp/če, jiná stavba, na parcele 267/9 Kunratice</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>budova na parcele č.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>58793</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Hlavní město Praha</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2428/21</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Kunratice</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>č. 2428/21 Kunratice</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>číslo a KU za ním</t>
         </is>

</xml_diff>

<commit_message>
Uprava vykreslovani do mapy, p[ridan tooltip
</commit_message>
<xml_diff>
--- a/GIS2/vystup.xlsx
+++ b/GIS2/vystup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,31 +477,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>58842</v>
+        <v>47800</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>jednotka</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1044/2</t>
+          <t>st. 646</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>č. 1044/2 Libuš</t>
+          <t>jednotka č. 4680004, byt v budově č.p. 468, 467, 469, část obce Olešovice, na parcele st. 646 Ládví, podíl na společných částech domu a pozemku 7596/110533</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -509,37 +509,37 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>jednotka na parcele s prefixem st. + KU</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>58841</v>
+        <v>47799</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1044/4</t>
+          <t>748/43</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>č. 1044/4 Libuš (součástí je stavba č.p. 957, čst obce Libuš)</t>
+          <t>č. 748/43 Ládví</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -547,37 +547,37 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>58840</v>
+        <v>47798</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1087/2</t>
+          <t>st. 334</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>č. 1087/2 Libuš</t>
+          <t>stavební č. 334 Ládví (součástí je stavba č.p. 154, čst obce Ládví)</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -585,13 +585,13 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>58839</v>
+        <v>47797</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -600,22 +600,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1088</t>
+          <t>125/12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>č. 1088 Libuš</t>
+          <t>č. 125/12 Ládví</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -629,7 +629,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>58838</v>
+        <v>47796</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -638,22 +638,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1087/1</t>
+          <t>st. 1372</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>č. 1087/1 Libuš (součástí je stavba č.p. 435, čst obce Libuš)</t>
+          <t>stavební č. 1372 Ládví (součástí je stavba budova bez čp/če, jiná stavba)</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -667,31 +667,31 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>58837</v>
+        <v>47795</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>546/1</t>
+          <t>st. 514</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>č. 546/1 Libuš</t>
+          <t>stavební č. 514 Ládví (součástí je stavba č.e. 1347, čst obce Ládví)</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -699,13 +699,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>58836</v>
+        <v>47794</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -714,22 +714,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>546/3</t>
+          <t>255/8</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>č. 546/3 Libuš</t>
+          <t>č. 255/8 Ládví</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -743,31 +743,31 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>58835</v>
+        <v>47793</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>546/2</t>
+          <t>722/12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>č. 546/2 Libuš (součástí je stavba budova bez čp/če, jiná stavba)</t>
+          <t>č. 722/12 Ládví</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -775,37 +775,37 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>58834</v>
+        <v>47792</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>546/4</t>
+          <t>234/4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>č. 546/4 Libuš (součástí je stavba budova bez čp/če, jiná stavba)</t>
+          <t>č. 234/4 Ládví</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -813,13 +813,13 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>58833</v>
+        <v>47791</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -828,22 +828,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>835/84</t>
+          <t>646/32</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>č. 835/84 Písnice</t>
+          <t>č. 646/32 Ládví</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -857,31 +857,31 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>58832</v>
+        <v>47790</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>761</t>
+          <t>st. 877</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>č. 761 Písnice</t>
+          <t>stavební č. 877 Ládví (součástí je stavba č.p. 1425, čst obce Olešovice)</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -889,37 +889,37 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>58831</v>
+        <v>47789</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>628/4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>č. 760 Písnice (součástí je stavba č.p. 329, čst obce Písnice)</t>
+          <t>č. 628/4 Ládví</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -927,37 +927,37 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>58830</v>
+        <v>47788</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>910/2</t>
+          <t>628/33</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>č. 628/33 Ládví</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -965,13 +965,13 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>jednotka na parcele bez prefixu st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>58830</v>
+        <v>47787</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -980,22 +980,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>910/3</t>
+          <t>st. 1313</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>jednotka č. 24010022, byt v budově č.p. 2401, část obce Olešovice, na parcele st. 1313 Ládví (součástí je stavba č.p. 2401, čst obce Olešovice), podíl na společných částech domu a pozemku 458/4518</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1003,37 +1003,37 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>jednotka na parcele s prefixem st. + KU</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>58830</v>
+        <v>47786</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>910/4</t>
+          <t>634/4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>č. 634/4 Ládví</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1041,37 +1041,37 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>58830</v>
+        <v>47785</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>910/5</t>
+          <t>634/5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>č. 634/5 Ládví</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1079,37 +1079,37 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>58830</v>
+        <v>47784</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>910/6</t>
+          <t>328/91</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>č. 328/91 Ládví</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1117,37 +1117,37 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>58830</v>
+        <v>47783</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>910/7</t>
+          <t>328/143</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>jednotka č. 3660007, byt v budově č.p. 361, 362, 363, 364, 365, 366, část obce Písnice, na parcele 910/2 Písnice (*), 910/3 Písnice (*), 910/4 Písnice (*), 910/5 Písnice (*), 910/6 Písnice (*), 910/7 Písnice, podíl na společných částech domu a pozemku 106/10000</t>
+          <t>č. 328/143 Ládví</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1155,13 +1155,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>58829</v>
+        <v>47782</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1170,22 +1170,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2197/2</t>
+          <t>414/49</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>č. 2197/2 Ledeč nad Sázavou</t>
+          <t>č. 414/49 Ládví</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1199,31 +1199,31 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>58828</v>
+        <v>47781</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>st. 500</t>
+          <t>414/48</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>stavební č. 500 Ledeč nad Sázavou (součástí je stavba č.p. 117, čst obce Horní Ledeč)</t>
+          <t>č. 414/48 Ládví</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1231,37 +1231,37 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>58827</v>
+        <v>47780</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>st. 825</t>
+          <t>st. 1294</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>jednotka č. 6450002, byt v budově č.p. 645, 646, část obce Ledeč nad Sázavou, na parcele st. 825 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 237/12278</t>
+          <t>stavební č. 1294 Ládví (součástí je stavba budova bez čp/če, garáž)</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1269,13 +1269,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>58826</v>
+        <v>47779</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1284,22 +1284,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2090/24</t>
+          <t>95/15</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>č. 2090/24 Ledeč nad Sázavou</t>
+          <t>č. 95/15 Ládví</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1313,31 +1313,31 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>58825</v>
+        <v>47778</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>st. 614</t>
+          <t>96/5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>jednotka č. 5540005, byt v budově č.p. 553, 554, část obce Ledeč nad Sázavou, na parcele st. 614 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 629/8741</t>
+          <t>č. 96/5 Ládví</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1345,37 +1345,37 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>58824</v>
+        <v>47777</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>st. 722</t>
+          <t>97/10</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>jednotka č. 6700007, byt v budově č.p. 670, část obce Ledeč nad Sázavou, na parcele st. 722 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 52/1000</t>
+          <t>č. 97/10 Ládví</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1383,37 +1383,37 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>58823</v>
+        <v>47776</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>823/5</t>
+          <t>st. 1315</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>č. 823/5 Ledeč nad Sázavou</t>
+          <t>stavební č. 1315 Ládví (součástí je stavba č.p. 2132, čst obce Ládví)</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1421,13 +1421,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>58822</v>
+        <v>47775</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1436,22 +1436,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>823/25</t>
+          <t>511/4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>č. 823/25 Ledeč nad Sázavou</t>
+          <t>č. 511/4 Ládví</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1465,7 +1465,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>58821</v>
+        <v>47774</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1474,22 +1474,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>823/32</t>
+          <t>103/17</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>č. 823/32 Ledeč nad Sázavou</t>
+          <t>č. 103/17 Ládví</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1503,31 +1503,31 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>58820</v>
+        <v>47773</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>st. 1640</t>
+          <t>27/10</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>stavební č. 1640 Ledeč nad Sázavou (součástí je stavba budova bez čp/če, garáž)</t>
+          <t>č. 27/10 Ládví</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1535,37 +1535,37 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>58819</v>
+        <v>47772</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>st. 710/2</t>
+          <t>103/16</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>stavební č. 710/2 Ledeč nad Sázavou (součástí je stavba budova bez čp/če, jiná stavba)</t>
+          <t>č. 103/16 Ládví</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1573,37 +1573,37 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>58818</v>
+        <v>47771</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>budova</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>st. 710/1</t>
+          <t>103/12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>stavební č. 710/1 Ledeč nad Sázavou (součástí je stavba č.p. 674, čst obce Ledeč nad Sázavou)</t>
+          <t>č. 103/12 Ládví</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1611,13 +1611,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>č. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>58817</v>
+        <v>47770</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1626,22 +1626,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>964</t>
+          <t>102/8</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>č. 964 Ledeč nad Sázavou</t>
+          <t>č. 102/8 Ládví</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1655,31 +1655,31 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>58816</v>
+        <v>47769</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Havlíčkův Brod</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>st. 601</t>
+          <t>103/10</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Ledeč nad Sázavou</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>jednotka č. 5560004, byt v budově č.p. 557, 555, 556, část obce Ledeč nad Sázavou, na parcele st. 601 Ledeč nad Sázavou, podíl na společných částech domu a pozemku 519/9693</t>
+          <t>č. 103/10 Ládví</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1687,37 +1687,37 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>jednotka na parcele s prefixem st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>58815</v>
+        <v>47768</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>429/48</t>
+          <t>103/13</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>jednotka č. 9860006, garáž v budově č.p. 986, část obce Libuš, na parcele 429/48 Libuš, podíl na společných částech domu a pozemku 184814/679789</t>
+          <t>č. 103/13 Ládví</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1725,13 +1725,13 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>jednotka na parcele bez prefixu st. + KU</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>58814</v>
+        <v>47767</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1740,22 +1740,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>429/48</t>
+          <t>st. 118</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>jednotka č. 9860410, byt v budově č.p. 986, část obce Libuš, na parcele 429/48 Libuš, podíl na společných částech domu a pozemku 5732/679789</t>
+          <t>jednotka č. 11480029, byt v budově č.p. 1148, část obce Ládví, na parcele st. 118 Ládví, podíl na společných částech domu a pozemku 732/32916</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1763,13 +1763,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>jednotka na parcele bez prefixu st. + KU</t>
+          <t>jednotka na parcele s prefixem st. + KU</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>58813</v>
+        <v>47766</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1778,22 +1778,22 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1123/116</t>
+          <t>364/36</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>č. 1123/116 Libuš</t>
+          <t>č. 364/36 Ládví</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1807,7 +1807,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>58812</v>
+        <v>47765</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1816,22 +1816,22 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1123/76</t>
+          <t>798</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>č. 1123/76 Libuš</t>
+          <t>č. 798 Ládví</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1845,7 +1845,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>58811</v>
+        <v>47764</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1854,22 +1854,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1123/73</t>
+          <t>618/9</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>č. 1123/73 Libuš</t>
+          <t>č. 618/9 Ládví</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1883,31 +1883,31 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>58810</v>
+        <v>47763</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>parcela</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1123/120</t>
+          <t>st. 931</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>č. 1123/120 Libuš</t>
+          <t>stavební č. 931 Ládví (součástí je stavba č.p. 1434, čst obce Olešovice)</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1915,13 +1915,13 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>číslo a KU za ním</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>58809</v>
+        <v>47762</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1930,22 +1930,22 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1123/118</t>
+          <t>578/3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>č. 1123/118 Libuš</t>
+          <t>č. 578/3 Ládví</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1959,7 +1959,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>58808</v>
+        <v>47761</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1968,22 +1968,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1123/119</t>
+          <t>578/2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>č. 1123/119 Libuš</t>
+          <t>č. 578/2 Ládví</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1997,7 +1997,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>58807</v>
+        <v>47760</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -2006,22 +2006,22 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1123/117</t>
+          <t>578/1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>č. 1123/117 Libuš</t>
+          <t>č. 578/1 Ládví</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -2035,7 +2035,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>58806</v>
+        <v>47759</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2044,22 +2044,22 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2382/8</t>
+          <t>340/1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>č. 2382/8 Kunratice</t>
+          <t>č. 340/1 Ládví</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -2073,7 +2073,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>58805</v>
+        <v>47758</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2082,22 +2082,22 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2342/27</t>
+          <t>432/9</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>č. 2342/27 Kunratice</t>
+          <t>č. 432/9 Ládví</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -2111,7 +2111,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>58804</v>
+        <v>47757</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2120,22 +2120,22 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2342/30</t>
+          <t>432/8</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>č. 2342/30 Kunratice</t>
+          <t>č. 432/8 Ládví</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2149,7 +2149,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>58803</v>
+        <v>47756</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2158,22 +2158,22 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2342/28</t>
+          <t>430/2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>č. 2342/28 Kunratice</t>
+          <t>č. 430/2 Ládví</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2187,7 +2187,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>58802</v>
+        <v>47755</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2196,22 +2196,22 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2342/29</t>
+          <t>459/9</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>č. 2342/29 Kunratice</t>
+          <t>č. 459/9 Ládví</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2225,7 +2225,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>58801</v>
+        <v>47754</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2234,22 +2234,22 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2342/31</t>
+          <t>st. 1186</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>č. 2342/31 Kunratice</t>
+          <t>stavební č. 1186 Ládví (součástí je stavba budova bez čp/če, jiná stavba)</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2263,31 +2263,31 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>58800</v>
+        <v>47753</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2342/27</t>
+          <t>st. 476</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+          <t>stavební č. 476 Ládví (součástí je stavba č.e. 1424, čst obce Ládví)</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2295,37 +2295,37 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>jednotka na parcele bez prefixu st. + KU</t>
+          <t>č. + KU</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>58800</v>
+        <v>47752</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>parcela</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2342/28</t>
+          <t>519/1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+          <t>č. 519/1 Ládví</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2333,37 +2333,37 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
+          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>58800</v>
+        <v>47751</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>jednotka</t>
+          <t>budova</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2342/29</t>
+          <t>st. 128</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
+          <t>stavební č. 128 Ládví (součástí je stavba č.e. 1485, čst obce Ládví)</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2371,501 +2371,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>58800</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>2342/30</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>58800</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>2342/31</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500902, garáž v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 17/7754</t>
-        </is>
-      </c>
-      <c r="G53" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>58799</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>2342/27</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
-        </is>
-      </c>
-      <c r="G54" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>jednotka na parcele bez prefixu st. + KU</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>58799</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2342/28</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
-        </is>
-      </c>
-      <c r="G55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>58799</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>2342/29</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
-        </is>
-      </c>
-      <c r="G56" t="n">
-        <v>1</v>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>58799</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2342/30</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
-        </is>
-      </c>
-      <c r="G57" t="n">
-        <v>1</v>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>58799</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>jednotka</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>2342/31</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>jednotka č. 11500061, byt v budově č.p. 1152, 1148, 1149, 1150, 1151, část obce Kunratice, na parcele 2342/27 Kunratice, 2342/28 Kunratice, 2342/29 Kunratice, 2342/30 Kunratice, 2342/31 Kunratice, podíl na společných částech domu a pozemku 82/7754</t>
-        </is>
-      </c>
-      <c r="G58" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>více parcel oddělených čárkou</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>58798</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>parcela</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>1433/13</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>č. 1433/13 Kunratice</t>
-        </is>
-      </c>
-      <c r="G59" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>číslo a KU za ním</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>58797</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>parcela</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>1433/12</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>č. 1433/12 Kunratice</t>
-        </is>
-      </c>
-      <c r="G60" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>číslo a KU za ním</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>58796</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>parcela</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>59/12</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>č. 59/12 Kunratice</t>
-        </is>
-      </c>
-      <c r="G61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>číslo a KU za ním</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>58795</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>budova</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>59/45</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>č. 59/45 Kunratice (součástí je stavba č.p. 1045, čst obce Kunratice)</t>
-        </is>
-      </c>
-      <c r="G62" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
           <t>č. + KU</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>58794</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>budova</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>267/9</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>budova bez čp/če, jiná stavba, na parcele 267/9 Kunratice</t>
-        </is>
-      </c>
-      <c r="G63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>budova na parcele č.</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>58793</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>parcela</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Hlavní město Praha</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>2428/21</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Kunratice</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>č. 2428/21 Kunratice</t>
-        </is>
-      </c>
-      <c r="G64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>číslo a KU za ním</t>
         </is>
       </c>
     </row>

</xml_diff>